<commit_message>
Updating AIC and RDA figures for manuscript, fixed mistake on RDA figure and created an optimal order 2 ODLM figure
</commit_message>
<xml_diff>
--- a/ODLM - AIC.xlsx
+++ b/ODLM - AIC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Box Sync\Hort Farm Experiment\2020 Benthic Pelagic Experiment\Tyler Hort Resilience\hort-benthic-pelagic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tjbut\Box Sync\Hort Farm Experiment\2020 Benthic Pelagic Experiment\Tyler Hort Resilience\hort-benthic-pelagic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABE5F8F9-9EB2-4DA5-BB56-383B4A12329D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BCC5033-262C-4B6D-AC58-3020152E32B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{90F1059C-7723-4C09-968D-9F89A9602C0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{90F1059C-7723-4C09-968D-9F89A9602C0B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A2:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>